<commit_message>
Changing code to use gemini
</commit_message>
<xml_diff>
--- a/kpi.xlsx
+++ b/kpi.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:X9"/>
+  <dimension ref="A1:X6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -441,7 +441,7 @@
       </c>
       <c r="B1" s="1" t="inlineStr">
         <is>
-          <t>cik</t>
+          <t>accession_number</t>
         </is>
       </c>
       <c r="C1" s="1" t="inlineStr">
@@ -558,7 +558,7 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>not specified</t>
+          <t>PRAX</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
@@ -578,37 +578,37 @@
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>Phase 2b</t>
+          <t>Phase 2a</t>
         </is>
       </c>
       <c r="F2" t="inlineStr">
         <is>
-          <t>Essential 1 study</t>
+          <t>NCT05021978</t>
         </is>
       </c>
       <c r="G2" t="inlineStr">
         <is>
-          <t>130</t>
+          <t>not specified</t>
         </is>
       </c>
       <c r="H2" t="inlineStr">
         <is>
-          <t>E</t>
+          <t>A</t>
         </is>
       </c>
       <c r="I2" t="inlineStr">
         <is>
-          <t>2023Q1</t>
+          <t>2022</t>
         </is>
       </c>
       <c r="J2" t="inlineStr">
         <is>
-          <t>Topline results expected for the ongoing Phase 2b Essential 1 study in Essential Tremor.</t>
+          <t>Demonstrated positive results in the study.</t>
         </is>
       </c>
       <c r="K2" t="inlineStr">
         <is>
-          <t>not specified</t>
+          <t>Positive</t>
         </is>
       </c>
       <c r="L2" t="inlineStr">
@@ -628,7 +628,7 @@
       </c>
       <c r="O2" t="inlineStr">
         <is>
-          <t>randomized, double-blind, placebo-controlled</t>
+          <t>not specified</t>
         </is>
       </c>
       <c r="P2" t="inlineStr">
@@ -638,7 +638,7 @@
       </c>
       <c r="Q2" t="inlineStr">
         <is>
-          <t>Placebo</t>
+          <t>not specified</t>
         </is>
       </c>
       <c r="R2" t="inlineStr">
@@ -663,24 +663,24 @@
       </c>
       <c r="V2" t="inlineStr">
         <is>
-          <t>not specified</t>
+          <t>positive results</t>
         </is>
       </c>
       <c r="W2" t="inlineStr">
         <is>
-          <t>Topline</t>
+          <t>not specified</t>
         </is>
       </c>
       <c r="X2" t="inlineStr">
         <is>
-          <t>Ongoing</t>
+          <t>Completed</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>not specified</t>
+          <t>PRAX</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
@@ -700,32 +700,32 @@
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>Phase 3</t>
+          <t>Phase 2b</t>
         </is>
       </c>
       <c r="F3" t="inlineStr">
         <is>
-          <t>Essential 3 trial</t>
+          <t>Essential 1</t>
         </is>
       </c>
       <c r="G3" t="inlineStr">
         <is>
-          <t>not specified</t>
+          <t>Approximately 130</t>
         </is>
       </c>
       <c r="H3" t="inlineStr">
         <is>
-          <t>E</t>
+          <t>A</t>
         </is>
       </c>
       <c r="I3" t="inlineStr">
         <is>
-          <t>2024H2</t>
+          <t>2023Q1</t>
         </is>
       </c>
       <c r="J3" t="inlineStr">
         <is>
-          <t>Topline results expected for the ongoing Phase 3 Essential 3 trial in Essential Tremor.</t>
+          <t>Topline results from the Essential 1 study were announced. The study is a multi-center, randomized, double-blind, placebo-controlled, dose-range finding clinical trial evaluating the efficacy, safety and tolerability of once-daily treatment of ulixacaltamide compared to placebo.</t>
         </is>
       </c>
       <c r="K3" t="inlineStr">
@@ -750,7 +750,7 @@
       </c>
       <c r="O3" t="inlineStr">
         <is>
-          <t>decentralized, multi-study</t>
+          <t>multi-center, randomized, double-blind, placebo-controlled, dose-range finding</t>
         </is>
       </c>
       <c r="P3" t="inlineStr">
@@ -760,7 +760,7 @@
       </c>
       <c r="Q3" t="inlineStr">
         <is>
-          <t>not specified</t>
+          <t>Placebo</t>
         </is>
       </c>
       <c r="R3" t="inlineStr">
@@ -770,7 +770,7 @@
       </c>
       <c r="S3" t="inlineStr">
         <is>
-          <t>NDA</t>
+          <t>not specified</t>
         </is>
       </c>
       <c r="T3" t="inlineStr">
@@ -795,14 +795,14 @@
       </c>
       <c r="X3" t="inlineStr">
         <is>
-          <t>Ongoing</t>
+          <t>Completed</t>
         </is>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>not specified</t>
+          <t>PRAX</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
@@ -817,7 +817,7 @@
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>Parkinson's Disease</t>
+          <t>Parkinson’s disease</t>
         </is>
       </c>
       <c r="E4" t="inlineStr">
@@ -847,7 +847,7 @@
       </c>
       <c r="J4" t="inlineStr">
         <is>
-          <t>Topline results expected for the Phase 2 trial in Parkinson's Disease.</t>
+          <t>A randomized, double-blind, placebo-controlled proof of concept trial planned to evaluate the efficacy, safety, and tolerability of ulixacaltamide as a non-dopaminergic treatment for motor symptoms of PD. Primary endpoint is change in UPDRS Part III motor examination score in the OFF state.</t>
         </is>
       </c>
       <c r="K4" t="inlineStr">
@@ -907,7 +907,7 @@
       </c>
       <c r="V4" t="inlineStr">
         <is>
-          <t>not specified</t>
+          <t>non-dopaminergic treatment for motor symptoms</t>
         </is>
       </c>
       <c r="W4" t="inlineStr">
@@ -917,14 +917,14 @@
       </c>
       <c r="X4" t="inlineStr">
         <is>
-          <t>Planned</t>
+          <t>not specified</t>
         </is>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>not specified</t>
+          <t>PRAX</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
@@ -939,22 +939,22 @@
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>Essential 1</t>
+          <t>Essential Tremor</t>
         </is>
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>Phase 2b</t>
+          <t>Phase 3</t>
         </is>
       </c>
       <c r="F5" t="inlineStr">
         <is>
-          <t>Essential 1 clinical trial</t>
+          <t>Essential 3 (Study 1 interim analysis)</t>
         </is>
       </c>
       <c r="G5" t="inlineStr">
         <is>
-          <t>not specified</t>
+          <t>N=400</t>
         </is>
       </c>
       <c r="H5" t="inlineStr">
@@ -964,17 +964,17 @@
       </c>
       <c r="I5" t="inlineStr">
         <is>
-          <t>2023Q1</t>
+          <t>2025Q1</t>
         </is>
       </c>
       <c r="J5" t="inlineStr">
         <is>
-          <t>Topline results from the Phase 2b Essential 1 clinical trial in essential tremor were announced.</t>
+          <t>Results of a pre-planned interim analysis of Study 1 of the Essential 3 clinical program were shared in February 2025. The IDMC recommended stopping for futility due to results being unlikely to meet the primary efficacy endpoint. The company decided to continue both studies to completion.</t>
         </is>
       </c>
       <c r="K5" t="inlineStr">
         <is>
-          <t>not specified</t>
+          <t>Futility</t>
         </is>
       </c>
       <c r="L5" t="inlineStr">
@@ -994,7 +994,7 @@
       </c>
       <c r="O5" t="inlineStr">
         <is>
-          <t>not specified</t>
+          <t>decentralized, multi-study, 12-week parallel design, placebo-controlled study</t>
         </is>
       </c>
       <c r="P5" t="inlineStr">
@@ -1004,7 +1004,7 @@
       </c>
       <c r="Q5" t="inlineStr">
         <is>
-          <t>not specified</t>
+          <t>Placebo</t>
         </is>
       </c>
       <c r="R5" t="inlineStr">
@@ -1034,19 +1034,19 @@
       </c>
       <c r="W5" t="inlineStr">
         <is>
-          <t>Topline</t>
+          <t>Interim</t>
         </is>
       </c>
       <c r="X5" t="inlineStr">
         <is>
-          <t>not specified</t>
+          <t>Ongoing</t>
         </is>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>not specified</t>
+          <t>PRAX</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
@@ -1061,7 +1061,7 @@
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>Essential 3</t>
+          <t>Essential Tremor</t>
         </is>
       </c>
       <c r="E6" t="inlineStr">
@@ -1071,12 +1071,12 @@
       </c>
       <c r="F6" t="inlineStr">
         <is>
-          <t>Essential 3 clinical trials</t>
+          <t>Essential 3 (Study 1 and Study 2 combined)</t>
         </is>
       </c>
       <c r="G6" t="inlineStr">
         <is>
-          <t>not specified</t>
+          <t>600</t>
         </is>
       </c>
       <c r="H6" t="inlineStr">
@@ -1086,12 +1086,12 @@
       </c>
       <c r="I6" t="inlineStr">
         <is>
-          <t>2024H2</t>
+          <t>2025Q3</t>
         </is>
       </c>
       <c r="J6" t="inlineStr">
         <is>
-          <t>Topline results from the ongoing Phase 3 Essential 3 clinical trials in essential tremor are expected.</t>
+          <t>Topline results for both Study 1 and Study 2 of the Essential 3 program are expected. A decision about whether the data supports NDA submission will be made after analyzing the final results.</t>
         </is>
       </c>
       <c r="K6" t="inlineStr">
@@ -1106,7 +1106,7 @@
       </c>
       <c r="M6" t="inlineStr">
         <is>
-          <t>not specified</t>
+          <t>Potential NDA submission in 2025</t>
         </is>
       </c>
       <c r="N6" t="inlineStr">
@@ -1116,7 +1116,7 @@
       </c>
       <c r="O6" t="inlineStr">
         <is>
-          <t>not specified</t>
+          <t>decentralized, multi-study, clinical trial evaluating safety and efficacy of 60 mg of ulixacaltamide in ET. Includes a 12-week parallel design, placebo-controlled study (Study 1) and a 12-week randomized withdrawal study (Study 2), with a long-term safety study (LTSS). Uses mADL11 as the primary endpoint.</t>
         </is>
       </c>
       <c r="P6" t="inlineStr">
@@ -1126,7 +1126,7 @@
       </c>
       <c r="Q6" t="inlineStr">
         <is>
-          <t>not specified</t>
+          <t>Placebo</t>
         </is>
       </c>
       <c r="R6" t="inlineStr">
@@ -1136,7 +1136,7 @@
       </c>
       <c r="S6" t="inlineStr">
         <is>
-          <t>not specified</t>
+          <t>NDA</t>
         </is>
       </c>
       <c r="T6" t="inlineStr">
@@ -1161,373 +1161,7 @@
       </c>
       <c r="X6" t="inlineStr">
         <is>
-          <t>not specified</t>
-        </is>
-      </c>
-    </row>
-    <row r="7">
-      <c r="A7" t="inlineStr">
-        <is>
-          <t>not specified</t>
-        </is>
-      </c>
-      <c r="B7" t="inlineStr">
-        <is>
-          <t>not specified</t>
-        </is>
-      </c>
-      <c r="C7" t="inlineStr">
-        <is>
-          <t>elsunersen</t>
-        </is>
-      </c>
-      <c r="D7" t="inlineStr">
-        <is>
-          <t>Solidus™ platform</t>
-        </is>
-      </c>
-      <c r="E7" t="inlineStr">
-        <is>
-          <t>not specified</t>
-        </is>
-      </c>
-      <c r="F7" t="inlineStr">
-        <is>
-          <t>EMBRAVE study</t>
-        </is>
-      </c>
-      <c r="G7" t="inlineStr">
-        <is>
-          <t>not specified</t>
-        </is>
-      </c>
-      <c r="H7" t="inlineStr">
-        <is>
-          <t>A</t>
-        </is>
-      </c>
-      <c r="I7" t="inlineStr">
-        <is>
-          <t>2023Q4</t>
-        </is>
-      </c>
-      <c r="J7" t="inlineStr">
-        <is>
-          <t>Results from Part 1 of the EMBRAVE study were shared in Q4 2023. Multiple global regulatory interactions are ongoing in anticipation of starting the pivotal phase later in 2024.</t>
-        </is>
-      </c>
-      <c r="K7" t="inlineStr">
-        <is>
-          <t>not specified</t>
-        </is>
-      </c>
-      <c r="L7" t="inlineStr">
-        <is>
-          <t>not specified</t>
-        </is>
-      </c>
-      <c r="M7" t="inlineStr">
-        <is>
-          <t>not specified</t>
-        </is>
-      </c>
-      <c r="N7" t="inlineStr">
-        <is>
-          <t>not specified</t>
-        </is>
-      </c>
-      <c r="O7" t="inlineStr">
-        <is>
-          <t>not specified</t>
-        </is>
-      </c>
-      <c r="P7" t="inlineStr">
-        <is>
-          <t>not specified</t>
-        </is>
-      </c>
-      <c r="Q7" t="inlineStr">
-        <is>
-          <t>not specified</t>
-        </is>
-      </c>
-      <c r="R7" t="inlineStr">
-        <is>
-          <t>not specified</t>
-        </is>
-      </c>
-      <c r="S7" t="inlineStr">
-        <is>
-          <t>not specified</t>
-        </is>
-      </c>
-      <c r="T7" t="inlineStr">
-        <is>
-          <t>not specified</t>
-        </is>
-      </c>
-      <c r="U7" t="inlineStr">
-        <is>
-          <t>not specified</t>
-        </is>
-      </c>
-      <c r="V7" t="inlineStr">
-        <is>
-          <t>not specified</t>
-        </is>
-      </c>
-      <c r="W7" t="inlineStr">
-        <is>
-          <t>not specified</t>
-        </is>
-      </c>
-      <c r="X7" t="inlineStr">
-        <is>
-          <t>not specified</t>
-        </is>
-      </c>
-    </row>
-    <row r="8">
-      <c r="A8" t="inlineStr">
-        <is>
-          <t>not specified</t>
-        </is>
-      </c>
-      <c r="B8" t="inlineStr">
-        <is>
-          <t>not specified</t>
-        </is>
-      </c>
-      <c r="C8" t="inlineStr">
-        <is>
-          <t>ulixacaltamide</t>
-        </is>
-      </c>
-      <c r="D8" t="inlineStr">
-        <is>
-          <t>Essential 3 Program</t>
-        </is>
-      </c>
-      <c r="E8" t="inlineStr">
-        <is>
-          <t>Phase 3</t>
-        </is>
-      </c>
-      <c r="F8" t="inlineStr">
-        <is>
-          <t>Study 1</t>
-        </is>
-      </c>
-      <c r="G8" t="inlineStr">
-        <is>
-          <t>400</t>
-        </is>
-      </c>
-      <c r="H8" t="inlineStr">
-        <is>
-          <t>E</t>
-        </is>
-      </c>
-      <c r="I8" t="inlineStr">
-        <is>
-          <t>2025Q3</t>
-        </is>
-      </c>
-      <c r="J8" t="inlineStr">
-        <is>
-          <t>The IDMC recommended stopping Study 1 for futility as results were unlikely to meet the primary efficacy endpoint. However, both Study 1 and Study 2 will continue to completion with topline results expected in Q3 2025.</t>
-        </is>
-      </c>
-      <c r="K8" t="inlineStr">
-        <is>
-          <t>Not Met</t>
-        </is>
-      </c>
-      <c r="L8" t="inlineStr">
-        <is>
-          <t>not specified</t>
-        </is>
-      </c>
-      <c r="M8" t="inlineStr">
-        <is>
-          <t>not specified</t>
-        </is>
-      </c>
-      <c r="N8" t="inlineStr">
-        <is>
-          <t>not specified</t>
-        </is>
-      </c>
-      <c r="O8" t="inlineStr">
-        <is>
-          <t>parallel design, placebo-controlled</t>
-        </is>
-      </c>
-      <c r="P8" t="inlineStr">
-        <is>
-          <t>not specified</t>
-        </is>
-      </c>
-      <c r="Q8" t="inlineStr">
-        <is>
-          <t>Placebo</t>
-        </is>
-      </c>
-      <c r="R8" t="inlineStr">
-        <is>
-          <t>not specified</t>
-        </is>
-      </c>
-      <c r="S8" t="inlineStr">
-        <is>
-          <t>not specified</t>
-        </is>
-      </c>
-      <c r="T8" t="inlineStr">
-        <is>
-          <t>not specified</t>
-        </is>
-      </c>
-      <c r="U8" t="inlineStr">
-        <is>
-          <t>not specified</t>
-        </is>
-      </c>
-      <c r="V8" t="inlineStr">
-        <is>
-          <t>not specified</t>
-        </is>
-      </c>
-      <c r="W8" t="inlineStr">
-        <is>
-          <t>Interim</t>
-        </is>
-      </c>
-      <c r="X8" t="inlineStr">
-        <is>
-          <t>not specified</t>
-        </is>
-      </c>
-    </row>
-    <row r="9">
-      <c r="A9" t="inlineStr">
-        <is>
-          <t>not specified</t>
-        </is>
-      </c>
-      <c r="B9" t="inlineStr">
-        <is>
-          <t>not specified</t>
-        </is>
-      </c>
-      <c r="C9" t="inlineStr">
-        <is>
-          <t>ulixacaltamide</t>
-        </is>
-      </c>
-      <c r="D9" t="inlineStr">
-        <is>
-          <t>Essential 3 Program</t>
-        </is>
-      </c>
-      <c r="E9" t="inlineStr">
-        <is>
-          <t>Phase 3</t>
-        </is>
-      </c>
-      <c r="F9" t="inlineStr">
-        <is>
-          <t>Study 2</t>
-        </is>
-      </c>
-      <c r="G9" t="inlineStr">
-        <is>
-          <t>200</t>
-        </is>
-      </c>
-      <c r="H9" t="inlineStr">
-        <is>
-          <t>E</t>
-        </is>
-      </c>
-      <c r="I9" t="inlineStr">
-        <is>
-          <t>2025Q3</t>
-        </is>
-      </c>
-      <c r="J9" t="inlineStr">
-        <is>
-          <t>Study 2 is part of the Essential 3 Program and will continue to completion with topline results expected in Q3 2025.</t>
-        </is>
-      </c>
-      <c r="K9" t="inlineStr">
-        <is>
-          <t>not specified</t>
-        </is>
-      </c>
-      <c r="L9" t="inlineStr">
-        <is>
-          <t>not specified</t>
-        </is>
-      </c>
-      <c r="M9" t="inlineStr">
-        <is>
-          <t>not specified</t>
-        </is>
-      </c>
-      <c r="N9" t="inlineStr">
-        <is>
-          <t>not specified</t>
-        </is>
-      </c>
-      <c r="O9" t="inlineStr">
-        <is>
-          <t>randomized withdrawal study</t>
-        </is>
-      </c>
-      <c r="P9" t="inlineStr">
-        <is>
-          <t>not specified</t>
-        </is>
-      </c>
-      <c r="Q9" t="inlineStr">
-        <is>
-          <t>not specified</t>
-        </is>
-      </c>
-      <c r="R9" t="inlineStr">
-        <is>
-          <t>not specified</t>
-        </is>
-      </c>
-      <c r="S9" t="inlineStr">
-        <is>
-          <t>not specified</t>
-        </is>
-      </c>
-      <c r="T9" t="inlineStr">
-        <is>
-          <t>not specified</t>
-        </is>
-      </c>
-      <c r="U9" t="inlineStr">
-        <is>
-          <t>not specified</t>
-        </is>
-      </c>
-      <c r="V9" t="inlineStr">
-        <is>
-          <t>not specified</t>
-        </is>
-      </c>
-      <c r="W9" t="inlineStr">
-        <is>
-          <t>not specified</t>
-        </is>
-      </c>
-      <c r="X9" t="inlineStr">
-        <is>
-          <t>not specified</t>
+          <t>Ongoing</t>
         </is>
       </c>
     </row>

</xml_diff>